<commit_message>
Changing mail to Gmail
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KamanProd\Input_files\Master_executors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36127F2-82A8-4AEF-9028-F79C0F5D622B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C4754A-909D-40F2-8CA8-016FFE36D194}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="MasterExecutor" sheetId="10" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MasterExecutor!$A$1:$F$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MasterExecutor!$A$1:$F$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="65">
   <si>
     <t>Functionality</t>
   </si>
@@ -236,13 +236,6 @@
   </si>
   <si>
     <t>Adding multiple items to cart in prod</t>
-  </si>
-  <si>
-    <t>TC02_Verify_HOME_PDP_PLP_CATEGORY</t>
-  </si>
-  <si>
-    <t>1. Go to home page
-2. Verify Home , PDP,PLP &amp; Category pages</t>
   </si>
 </sst>
 </file>
@@ -380,7 +373,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{A444948E-6AA8-45F3-AB40-38513383CF85}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -753,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E30"/>
+      <selection activeCell="E2" sqref="E2:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -808,7 +811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:6" ht="45">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -816,10 +819,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>59</v>
@@ -828,7 +831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -836,10 +839,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>59</v>
@@ -855,11 +858,11 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>59</v>
@@ -868,18 +871,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="45">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
+      <c r="C6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>59</v>
@@ -888,18 +891,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>55</v>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>59</v>
@@ -916,10 +919,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>59</v>
@@ -936,10 +939,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>59</v>
@@ -956,10 +959,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>59</v>
@@ -976,10 +979,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>59</v>
@@ -988,7 +991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -996,10 +999,10 @@
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>59</v>
@@ -1008,18 +1011,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>59</v>
@@ -1028,27 +1031,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:6" ht="30">
+      <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30">
+      <c r="F14" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1056,19 +1059,19 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="F15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1076,10 +1079,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>59</v>
@@ -1088,7 +1091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -1096,10 +1099,10 @@
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>59</v>
@@ -1116,9 +1119,9 @@
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -1136,10 +1139,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>59</v>
@@ -1156,10 +1159,10 @@
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>59</v>
@@ -1175,11 +1178,11 @@
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>50</v>
+      <c r="C21" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>59</v>
@@ -1196,15 +1199,15 @@
         <v>6</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1215,11 +1218,11 @@
       <c r="B23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>58</v>
+      <c r="C23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>59</v>
@@ -1229,17 +1232,17 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>59</v>
@@ -1256,10 +1259,10 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>59</v>
@@ -1276,10 +1279,10 @@
         <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>20</v>
+        <v>53</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>59</v>
@@ -1296,10 +1299,10 @@
         <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>59</v>
@@ -1308,18 +1311,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="7" t="s">
+    <row r="28" spans="1:6" ht="45">
+      <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>59</v>
@@ -1328,7 +1331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="45">
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -1336,46 +1339,26 @@
         <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F23:F29">
-    <cfRule type="uniqueValues" dxfId="2" priority="80"/>
+  <conditionalFormatting sqref="F22:F28">
+    <cfRule type="uniqueValues" dxfId="3" priority="81"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2 E4:E30">
-    <cfRule type="uniqueValues" dxfId="1" priority="83"/>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="uniqueValues" dxfId="2" priority="84"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
+  <conditionalFormatting sqref="E3:E29">
     <cfRule type="uniqueValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>